<commit_message>
Para producion - Testing
</commit_message>
<xml_diff>
--- a/public/excel/ventas-directas.xlsx
+++ b/public/excel/ventas-directas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Número</t>
   </si>
@@ -28,13 +28,13 @@
     <t>Precio total</t>
   </si>
   <si>
-    <t>MORENO LUCAS OMAR</t>
-  </si>
-  <si>
-    <t>CONSUMIDOR FINAL</t>
+    <t>Habilitada</t>
   </si>
   <si>
     <t>EQUINOCCIO TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -416,16 +416,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,247 +442,32 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>44827.93721105324</v>
+        <v>44876.86133134259</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2">
-        <v>36313.98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44827.93627959491</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>10065</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
-        <v>44825.889994513884</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
+        <v>5000</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
-      </c>
-      <c r="E4">
-        <v>15013.380000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
-        <v>44818.98116622685</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" s="2">
-        <v>44818.97592877314</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>3300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2">
-        <v>44818.9731697338</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>1950</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
-        <v>44818.97112203704</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>44818.96779815972</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>3400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" s="2">
-        <v>44818.96620494213</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <v>44815.85347952547</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>7100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" s="2">
-        <v>44815.8530105324</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12">
-        <v>4300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2">
-        <v>44815.78415155092</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2">
-        <v>44815.6917200926</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>44815.681656597226</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15">
-        <v>3000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>